<commit_message>
update file import company
</commit_message>
<xml_diff>
--- a/public/images/import-comany.xlsx
+++ b/public/images/import-comany.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Wiseman\OneDrive\Máy tính\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D20C801F-280C-44CE-8AF1-BAB0DADA889B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2B1D091-9721-476F-AADB-083FCB6665A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2811" yWindow="2811" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Tên công ty</t>
   </si>
@@ -60,20 +60,29 @@
     <t>Doctor Who</t>
   </si>
   <si>
-    <t>Công Ty Đầu Lâu</t>
-  </si>
-  <si>
     <t>0988444334</t>
   </si>
   <si>
     <t>Wang Dong Ping</t>
+  </si>
+  <si>
+    <t>Công Ty Lienketso</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>thanhan1507@gmail.com</t>
+  </si>
+  <si>
+    <t>who@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +94,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,10 +124,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -121,8 +139,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -401,10 +421,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -417,7 +437,7 @@
     <col min="6" max="6" width="13.765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
@@ -436,13 +456,16 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="5">
         <v>106120454</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="5">
         <v>2020</v>
@@ -451,13 +474,16 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
-        <v>13</v>
+      <c r="G2" s="6" t="s">
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>106120456</v>
       </c>
@@ -476,9 +502,16 @@
       <c r="F3" t="s">
         <v>10</v>
       </c>
+      <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{601255EB-9F69-47A8-AF59-D1430CA57E44}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{B5A1D699-01FF-4C24-ABD8-3740D150FD75}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>